<commit_message>
ebook exporter, dpd splitter, sandhi divide mula and rest, make words in sandhi set, foreign key default '', gui kn1 &kn2, gui bind enter key, family set fix, make mūla words set, cst sc lists, round bip bop
</commit_message>
<xml_diff>
--- a/inflections/inflection_templates.xlsx
+++ b/inflections/inflection_templates.xlsx
@@ -9638,7 +9638,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A102" activeCellId="0" sqref="A102"/>
-      <selection pane="bottomRight" activeCell="A121" activeCellId="0" sqref="A121"/>
+      <selection pane="bottomRight" activeCell="A121" activeCellId="1" sqref="BL32 A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -38875,8 +38875,8 @@
   </sheetPr>
   <dimension ref="A1:DK350"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CD140" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CK148" activeCellId="0" sqref="CK148"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AX25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BL32" activeCellId="0" sqref="BL32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -45038,7 +45038,7 @@
       <c r="CV31" s="20"/>
       <c r="CW31" s="20"/>
     </row>
-    <row r="32" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="22"/>
       <c r="B32" s="22"/>
       <c r="C32" s="49"/>
@@ -45082,7 +45082,7 @@
         <v>589</v>
       </c>
       <c r="BH32" s="42" t="s">
-        <v>812</v>
+        <v>805</v>
       </c>
       <c r="BI32" s="56" t="s">
         <v>591</v>
@@ -45091,7 +45091,7 @@
         <v>587</v>
       </c>
       <c r="BL32" s="42" t="s">
-        <v>812</v>
+        <v>805</v>
       </c>
       <c r="BM32" s="56" t="s">
         <v>591</v>
@@ -45106,7 +45106,7 @@
         <v>593</v>
       </c>
       <c r="BT32" s="28" t="s">
-        <v>812</v>
+        <v>805</v>
       </c>
       <c r="BU32" s="43" t="s">
         <v>595</v>
@@ -45115,7 +45115,7 @@
         <v>587</v>
       </c>
       <c r="BX32" s="28" t="s">
-        <v>812</v>
+        <v>805</v>
       </c>
       <c r="BY32" s="43" t="s">
         <v>595</v>
@@ -73586,7 +73586,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="bottomRight" activeCell="A19" activeCellId="1" sqref="BL32 A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -76036,7 +76036,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B201" activeCellId="0" sqref="B201"/>
+      <selection pane="bottomLeft" activeCell="B201" activeCellId="1" sqref="BL32 B201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.19921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
backup paliword & paliroot
</commit_message>
<xml_diff>
--- a/inflections/inflection_templates.xlsx
+++ b/inflections/inflection_templates.xlsx
@@ -9646,7 +9646,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A102" activeCellId="0" sqref="A102"/>
-      <selection pane="bottomRight" activeCell="A121" activeCellId="0" sqref="A121"/>
+      <selection pane="bottomRight" activeCell="A121" activeCellId="1" sqref="CN142 A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -38883,8 +38883,8 @@
   </sheetPr>
   <dimension ref="A1:DK350"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AW76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BF82" activeCellId="0" sqref="BF82"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CB134" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="CN142" activeCellId="0" sqref="CN142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -59203,7 +59203,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="23"/>
       <c r="D112" s="23"/>
       <c r="F112" s="23"/>
@@ -59255,7 +59255,7 @@
         <v>668</v>
       </c>
       <c r="CN112" s="57" t="s">
-        <v>416</v>
+        <v>1225</v>
       </c>
       <c r="CO112" s="58" t="s">
         <v>934</v>
@@ -63362,7 +63362,7 @@
       </c>
       <c r="DA141" s="48"/>
     </row>
-    <row r="142" customFormat="false" ht="69.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="22" t="s">
         <v>567</v>
       </c>
@@ -63471,7 +63471,7 @@
         <v>668</v>
       </c>
       <c r="CN142" s="57" t="s">
-        <v>416</v>
+        <v>1225</v>
       </c>
       <c r="CO142" s="58" t="s">
         <v>934</v>
@@ -73594,7 +73594,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="bottomRight" activeCell="A19" activeCellId="1" sqref="CN142 A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -76044,7 +76044,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B201" activeCellId="0" sqref="B201"/>
+      <selection pane="bottomLeft" activeCell="B201" activeCellId="1" sqref="CN142 B201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.19921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
sutta examples, pass2, update
</commit_message>
<xml_diff>
--- a/inflections/inflection_templates.xlsx
+++ b/inflections/inflection_templates.xlsx
@@ -6092,6 +6092,7 @@
   </si>
   <si>
     <t xml:space="preserve">aresu
+ū
 ūsu</t>
   </si>
   <si>
@@ -38912,8 +38913,8 @@
   </sheetPr>
   <dimension ref="A1:DK350"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BJ26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BR30" activeCellId="0" sqref="BR30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AW123" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BH131" activeCellId="0" sqref="BH131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -61275,7 +61276,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="50.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="22" t="s">
         <v>411</v>
       </c>

</xml_diff>